<commit_message>
Implement research kgrams Small changes
</commit_message>
<xml_diff>
--- a/StatsAboutTitles.xlsx
+++ b/StatsAboutTitles.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5b75b1c6a55d49cb/College/JuniorYear/CS5140/Grade Data Mining Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\North\OneDrive\College\JuniorYear\CS5140\Grade Data Mining Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA50AD4F-F278-4E71-90BB-1E5AFD34A4A7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{AA50AD4F-F278-4E71-90BB-1E5AFD34A4A7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{971295BE-FC4C-40B3-AE18-78E05658CAE3}"/>
   <bookViews>
-    <workbookView xWindow="5550" yWindow="5550" windowWidth="24900" windowHeight="11700" xr2:uid="{1222B20C-42B5-4AE8-A7B3-DD81D70E9383}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{1222B20C-42B5-4AE8-A7B3-DD81D70E9383}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,9 +48,6 @@
     <t>GPA</t>
   </si>
   <si>
-    <t>L1 Grade Vector</t>
-  </si>
-  <si>
     <t xml:space="preserve">Professor </t>
   </si>
   <si>
@@ -103,6 +100,9 @@
   </si>
   <si>
     <t xml:space="preserve"> [0.43243243243243246, 0.31756756756756754, 0.20945945945945946, 0.04054054054054054, 0.0, 0.0, 0.0]</t>
+  </si>
+  <si>
+    <t>Grade PDF</t>
   </si>
 </sst>
 </file>
@@ -456,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D1C3C65-FD18-4F1E-884E-2580878524BB}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScale="280" zoomScaleNormal="280" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,15 +485,15 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B2">
-        <v>321616</v>
+        <v>21897</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -502,18 +502,18 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B3">
-        <v>191890</v>
+        <v>465991</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -522,130 +522,130 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>2.875</v>
+        <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B4">
-        <v>148270.28571428501</v>
+        <v>249943</v>
       </c>
       <c r="C4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>2.9247774625843599</v>
+        <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5">
-        <v>239207.42105263099</v>
+        <v>150318.125</v>
       </c>
       <c r="C5">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>2.9621005299502099</v>
+        <v>3.1615384615384601</v>
       </c>
       <c r="F5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B6">
-        <v>172116.66666666599</v>
+        <v>158000</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>3.01391465677179</v>
+        <v>3.1418918918918899</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B7">
-        <v>158000</v>
+        <v>172116.66666666599</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>3.1418918918918899</v>
+        <v>3.01391465677179</v>
       </c>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B8">
-        <v>150318.125</v>
+        <v>239207.42105263099</v>
       </c>
       <c r="C8">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E8">
-        <v>3.1615384615384601</v>
+        <v>2.9621005299502099</v>
       </c>
       <c r="F8" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9">
-        <v>465991</v>
+        <v>148270.28571428501</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>4</v>
+        <v>2.9247774625843599</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -653,7 +653,7 @@
         <v>16</v>
       </c>
       <c r="B10">
-        <v>21897</v>
+        <v>191890</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -662,10 +662,10 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>4</v>
+        <v>2.875</v>
       </c>
       <c r="F10" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -673,7 +673,7 @@
         <v>19</v>
       </c>
       <c r="B11">
-        <v>249943</v>
+        <v>321616</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -682,16 +682,17 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F11">
-    <sortCondition ref="E1"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:F14">
+    <sortCondition descending="1" ref="E1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>